<commit_message>
final project part TP1
</commit_message>
<xml_diff>
--- a/gso-7085/instance_2.xlsx
+++ b/gso-7085/instance_2.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t># pièce</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>#2</t>
+  </si>
+  <si>
+    <t>#3</t>
   </si>
 </sst>
 </file>
@@ -464,7 +467,7 @@
   <dimension ref="A1:M212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,10 +571,25 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.5</v>
+      </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>

</xml_diff>

<commit_message>
nouvelle version du projet
</commit_message>
<xml_diff>
--- a/gso-7085/instance_2.xlsx
+++ b/gso-7085/instance_2.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t># pièce</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>#2</t>
-  </si>
-  <si>
-    <t>#3</t>
   </si>
 </sst>
 </file>
@@ -467,7 +464,7 @@
   <dimension ref="A1:M212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,16 +526,16 @@
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2">
-        <v>6</v>
-      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="3"/>
       <c r="E2">
-        <v>8</v>
+        <v>1.5</v>
       </c>
       <c r="F2" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>0.5</v>
@@ -549,47 +546,45 @@
         <v>18</v>
       </c>
       <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
         <v>5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>2</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>9</v>
+        <v>7.5</v>
       </c>
       <c r="F3" s="6">
+        <v>2</v>
+      </c>
+      <c r="G3" s="6">
         <v>1</v>
       </c>
-      <c r="G3" s="6">
+      <c r="H3" s="6">
         <v>2</v>
       </c>
       <c r="I3">
-        <v>0.5</v>
+        <v>0.8</v>
+      </c>
+      <c r="J3" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="K3" s="6">
+        <v>2</v>
+      </c>
+      <c r="L3" s="3">
+        <v>2.5</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1.5</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4" s="3">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0.5</v>
-      </c>
+      <c r="D4" s="3"/>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>

</xml_diff>